<commit_message>
generación de modelos para cada componente
</commit_message>
<xml_diff>
--- a/metadatos.xlsx
+++ b/metadatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damoib/Documents/Galileo/papd-proyecto-final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B59F8AF-109D-6649-A302-61914A398B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BFC397-8ECB-1B4E-B8FE-724B0ECEDF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="520" windowWidth="25600" windowHeight="26340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="227">
   <si>
     <t>sector</t>
   </si>
@@ -715,6 +715,9 @@
   <si>
     <t>$dif_tasa_var</t>
   </si>
+  <si>
+    <t>act_servicios</t>
+  </si>
 </sst>
 </file>
 
@@ -737,6 +740,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -744,6 +748,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -751,12 +756,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -764,12 +771,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -781,6 +790,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2466,15 +2476,15 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C173" sqref="C173"/>
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" customWidth="1"/>
-    <col min="3" max="3" width="86.6640625" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10534,7 +10544,7 @@
         <v>180</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>87</v>
+        <v>226</v>
       </c>
       <c r="D162" s="8" t="s">
         <v>14</v>
@@ -36731,7 +36741,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" ht="16">
       <c r="A1" s="24" t="s">
         <v>213</v>
       </c>
@@ -36772,7 +36782,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" ht="16">
       <c r="A2" s="26">
         <v>39994</v>
       </c>
@@ -36812,7 +36822,7 @@
         <v>319.3</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" ht="16">
       <c r="A3" s="26">
         <v>40086</v>
       </c>
@@ -36852,7 +36862,7 @@
         <v>-1913.4</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" ht="16">
       <c r="A4" s="28">
         <v>40178</v>
       </c>
@@ -36892,7 +36902,7 @@
         <v>488.9</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" ht="16">
       <c r="A5" s="26">
         <v>40268</v>
       </c>
@@ -36932,7 +36942,7 @@
         <v>-2758.6</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" ht="16">
       <c r="A6" s="26">
         <v>40359</v>
       </c>
@@ -36978,7 +36988,7 @@
         <v>192.4</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" ht="16">
       <c r="A7" s="26">
         <v>40451</v>
       </c>
@@ -37024,7 +37034,7 @@
         <v>-556.29999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" ht="16">
       <c r="A8" s="28">
         <v>40543</v>
       </c>
@@ -37070,7 +37080,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" ht="16">
       <c r="A9" s="26">
         <v>40633</v>
       </c>
@@ -37116,7 +37126,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" ht="16">
       <c r="A10" s="26">
         <v>40724</v>
       </c>
@@ -37162,7 +37172,7 @@
         <v>-61</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" ht="16">
       <c r="A11" s="26">
         <v>40816</v>
       </c>
@@ -37208,7 +37218,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" ht="16">
       <c r="A12" s="28">
         <v>40908</v>
       </c>
@@ -37254,7 +37264,7 @@
         <v>-24.3</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" ht="16">
       <c r="A13" s="26">
         <v>40999</v>
       </c>
@@ -37300,7 +37310,7 @@
         <v>3972.5</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" ht="16">
       <c r="A14" s="26">
         <v>41090</v>
       </c>
@@ -37346,7 +37356,7 @@
         <v>-818.7</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" ht="16">
       <c r="A15" s="26">
         <v>41182</v>
       </c>
@@ -37392,7 +37402,7 @@
         <v>-35.4</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" ht="16">
       <c r="A16" s="28">
         <v>41274</v>
       </c>
@@ -37438,7 +37448,7 @@
         <v>-656.9</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" ht="16">
       <c r="A17" s="26">
         <v>41364</v>
       </c>
@@ -37484,7 +37494,7 @@
         <v>4469.6499999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" ht="16">
       <c r="A18" s="26">
         <v>41455</v>
       </c>
@@ -37530,7 +37540,7 @@
         <v>-790.67</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" ht="16">
       <c r="A19" s="26">
         <v>41547</v>
       </c>
@@ -37576,7 +37586,7 @@
         <v>-258.31</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" ht="16">
       <c r="A20" s="28">
         <v>41639</v>
       </c>
@@ -37622,7 +37632,7 @@
         <v>-289.22000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" ht="16">
       <c r="A21" s="26">
         <v>41729</v>
       </c>
@@ -37668,7 +37678,7 @@
         <v>4024.46</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" ht="16">
       <c r="A22" s="26">
         <v>41820</v>
       </c>
@@ -37714,7 +37724,7 @@
         <v>-1282.53</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" ht="16">
       <c r="A23" s="26">
         <v>41912</v>
       </c>
@@ -37760,7 +37770,7 @@
         <v>-2026.75</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" ht="16">
       <c r="A24" s="28">
         <v>42004</v>
       </c>
@@ -37806,7 +37816,7 @@
         <v>-1157.78</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" ht="16">
       <c r="A25" s="26">
         <v>42094</v>
       </c>
@@ -37852,7 +37862,7 @@
         <v>3090.82</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" ht="16">
       <c r="A26" s="26">
         <v>42185</v>
       </c>
@@ -37898,7 +37908,7 @@
         <v>-601.9</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" ht="16">
       <c r="A27" s="26">
         <v>42277</v>
       </c>
@@ -37944,7 +37954,7 @@
         <v>40.450000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" ht="16">
       <c r="A28" s="28">
         <v>42369</v>
       </c>
@@ -37990,7 +38000,7 @@
         <v>-1030.54</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" ht="16">
       <c r="A29" s="26">
         <v>42460</v>
       </c>
@@ -38036,7 +38046,7 @@
         <v>2071.59</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" ht="16">
       <c r="A30" s="26">
         <v>42551</v>
       </c>
@@ -38082,7 +38092,7 @@
         <v>-381.37</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" ht="16">
       <c r="A31" s="26">
         <v>42643</v>
       </c>
@@ -38128,7 +38138,7 @@
         <v>-1314.82</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" ht="16">
       <c r="A32" s="28">
         <v>42735</v>
       </c>
@@ -38174,7 +38184,7 @@
         <v>-542.94000000000005</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" ht="16">
       <c r="A33" s="26">
         <v>42825</v>
       </c>
@@ -38220,7 +38230,7 @@
         <v>3590.27</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" ht="16">
       <c r="A34" s="26">
         <v>42916</v>
       </c>
@@ -38266,7 +38276,7 @@
         <v>-1292.92</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" ht="16">
       <c r="A35" s="26">
         <v>43008</v>
       </c>
@@ -38312,7 +38322,7 @@
         <v>-1960.35</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" ht="16">
       <c r="A36" s="28">
         <v>43100</v>
       </c>
@@ -38358,7 +38368,7 @@
         <v>-349.63</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" ht="16">
       <c r="A37" s="26">
         <v>43190</v>
       </c>
@@ -38404,7 +38414,7 @@
         <v>3876.83</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" ht="16">
       <c r="A38" s="26">
         <v>43281</v>
       </c>
@@ -38450,7 +38460,7 @@
         <v>33.909999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" ht="16">
       <c r="A39" s="26">
         <v>43373</v>
       </c>
@@ -38496,7 +38506,7 @@
         <v>-2227.87</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" ht="16">
       <c r="A40" s="28">
         <v>43465</v>
       </c>
@@ -38542,7 +38552,7 @@
         <v>-1005.42</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" ht="16">
       <c r="A41" s="26">
         <v>43555</v>
       </c>
@@ -38588,7 +38598,7 @@
         <v>4524.38</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" ht="16">
       <c r="A42" s="26">
         <v>43646</v>
       </c>
@@ -38634,7 +38644,7 @@
         <v>-1678.44</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" ht="16">
       <c r="A43" s="26">
         <v>43738</v>
       </c>
@@ -38680,7 +38690,7 @@
         <v>-2350.8200000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" ht="16">
       <c r="A44" s="28">
         <v>43830</v>
       </c>
@@ -38726,7 +38736,7 @@
         <v>-505.52</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" ht="16">
       <c r="A45" s="26">
         <v>43921</v>
       </c>
@@ -38772,7 +38782,7 @@
         <v>5216.8599999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" ht="16">
       <c r="A46" s="26">
         <v>44012</v>
       </c>
@@ -38818,7 +38828,7 @@
         <v>-1599.27</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" ht="16">
       <c r="A47" s="26">
         <v>44104</v>
       </c>
@@ -38864,7 +38874,7 @@
         <v>-3582.37</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" ht="16">
       <c r="A48" s="28">
         <v>44196</v>
       </c>
@@ -38910,7 +38920,7 @@
         <v>-986.12</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" ht="16">
       <c r="A49" s="26">
         <v>44286</v>
       </c>
@@ -38956,7 +38966,7 @@
         <v>3737.91</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" ht="16">
       <c r="A50" s="26">
         <v>44377</v>
       </c>
@@ -39002,7 +39012,7 @@
         <v>1093.32</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" ht="16">
       <c r="A51" s="26">
         <v>44469</v>
       </c>
@@ -39048,7 +39058,7 @@
         <v>-748.83</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" ht="16">
       <c r="A52" s="28">
         <v>44561</v>
       </c>
@@ -39094,7 +39104,7 @@
         <v>-125.78</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" ht="16">
       <c r="A53" s="26">
         <v>44651</v>
       </c>
@@ -39140,7 +39150,7 @@
         <v>4439.3</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" ht="16">
       <c r="A54" s="26">
         <v>44742</v>
       </c>
@@ -39186,7 +39196,7 @@
         <v>-719.76</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" ht="16">
       <c r="A55" s="26">
         <v>44834</v>
       </c>
@@ -39232,7 +39242,7 @@
         <v>-1248.99</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" ht="16">
       <c r="A56" s="28">
         <v>44926</v>
       </c>
@@ -39278,7 +39288,7 @@
         <v>-3919.86</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" ht="16">
       <c r="A57" s="26">
         <v>45016</v>
       </c>
@@ -39324,7 +39334,7 @@
         <v>1500.78</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" ht="16">
       <c r="A58" s="26">
         <v>45107</v>
       </c>
@@ -39370,7 +39380,7 @@
         <v>-602.86</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" ht="16">
       <c r="A59" s="26">
         <v>45199</v>
       </c>
@@ -39416,7 +39426,7 @@
         <v>435.9</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" ht="16">
       <c r="A60" s="28">
         <v>45291</v>
       </c>
@@ -39462,7 +39472,7 @@
         <v>1609.31</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" ht="16">
       <c r="A61" s="26">
         <v>45382</v>
       </c>
@@ -39508,7 +39518,7 @@
         <v>6899.95</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" ht="16">
       <c r="A62" s="26">
         <v>45473</v>
       </c>

</xml_diff>